<commit_message>
YA funciona toda la lógica del cliente, falta replicar de forma similar en empresa
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="50">
   <si>
     <t>CLIENTE</t>
   </si>
@@ -500,8 +500,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:F48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="D49" sqref="D49"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -624,86 +624,92 @@
       </c>
     </row>
     <row r="32" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C32" t="s">
+        <v>49</v>
+      </c>
       <c r="D32" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="33" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C33" t="s">
+        <v>49</v>
+      </c>
       <c r="D33" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="34" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D34" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="35" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D35" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="36" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D36" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="37" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D37" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="38" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D38" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="39" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D39" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="40" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D40" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="41" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D41" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="42" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D42" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="43" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D43" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="44" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D44" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="45" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D45" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="46" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D46" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="47" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D47" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="48" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D48" t="s">
         <v>48</v>
       </c>

</xml_diff>

<commit_message>
Falta darle estilos en perfiles de ambos usuarios, la lógica en general funciona, falta revisar la lógica de UX
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="51">
   <si>
     <t>CLIENTE</t>
   </si>
@@ -178,6 +178,9 @@
   </si>
   <si>
     <t>ok</t>
+  </si>
+  <si>
+    <t>Aparecer en vista arq</t>
   </si>
 </sst>
 </file>
@@ -500,8 +503,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:F48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="D48" sqref="D48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -631,7 +634,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="33" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C33" t="s">
         <v>49</v>
       </c>
@@ -639,77 +642,95 @@
         <v>33</v>
       </c>
     </row>
-    <row r="34" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C34" t="s">
+        <v>49</v>
+      </c>
       <c r="D34" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="35" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C35" t="s">
+        <v>49</v>
+      </c>
       <c r="D35" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="36" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C36" t="s">
+        <v>49</v>
+      </c>
       <c r="D36" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="37" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D37" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="38" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="E37" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="38" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C38" t="s">
+        <v>49</v>
+      </c>
       <c r="D38" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="39" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D39" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="40" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="E39" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="40" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D40" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="41" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D41" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="42" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D42" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="43" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D43" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="44" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D44" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="45" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D45" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="46" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D46" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="47" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D47" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="48" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D48" t="s">
         <v>48</v>
       </c>

</xml_diff>